<commit_message>
fix [admin] ajax penentuan lokasi
</commit_message>
<xml_diff>
--- a/public/AkunMahasiswa/cek.xlsx
+++ b/public/AkunMahasiswa/cek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC5E736-34E8-428E-B6BC-233F9C65C880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CCEF28-6A51-4D06-94F1-66EA1BA4EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{0A5A482C-4977-4C35-8E96-A3B76D5000BF}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>